<commit_message>
revert to legacy capInfo elec order but reorder loc file to match capInfo order
</commit_message>
<xml_diff>
--- a/capInfo.xlsx
+++ b/capInfo.xlsx
@@ -18,262 +18,262 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="984" uniqueCount="984">
   <si>
+    <t>LPA</t>
+  </si>
+  <si>
+    <t>RPA</t>
+  </si>
+  <si>
+    <t>Nz</t>
+  </si>
+  <si>
     <t>Fp1</t>
   </si>
   <si>
+    <t>Fpz</t>
+  </si>
+  <si>
     <t>Fp2</t>
   </si>
   <si>
+    <t>AF7</t>
+  </si>
+  <si>
+    <t>AF5</t>
+  </si>
+  <si>
+    <t>AF3</t>
+  </si>
+  <si>
+    <t>AF1</t>
+  </si>
+  <si>
+    <t>AFz</t>
+  </si>
+  <si>
+    <t>AF2</t>
+  </si>
+  <si>
+    <t>AF4</t>
+  </si>
+  <si>
+    <t>AF6</t>
+  </si>
+  <si>
+    <t>AF8</t>
+  </si>
+  <si>
+    <t>F9</t>
+  </si>
+  <si>
+    <t>F7</t>
+  </si>
+  <si>
+    <t>F5</t>
+  </si>
+  <si>
     <t>F3</t>
   </si>
   <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>Fz</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
     <t>F4</t>
   </si>
   <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
+    <t>F10</t>
+  </si>
+  <si>
+    <t>FT9</t>
+  </si>
+  <si>
+    <t>FT7</t>
+  </si>
+  <si>
+    <t>FC5</t>
+  </si>
+  <si>
+    <t>FC3</t>
+  </si>
+  <si>
+    <t>FC1</t>
+  </si>
+  <si>
+    <t>FCz</t>
+  </si>
+  <si>
+    <t>FC2</t>
+  </si>
+  <si>
+    <t>FC4</t>
+  </si>
+  <si>
+    <t>FC6</t>
+  </si>
+  <si>
+    <t>FT8</t>
+  </si>
+  <si>
+    <t>FT10</t>
+  </si>
+  <si>
+    <t>T9</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
     <t>C3</t>
   </si>
   <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>Cz</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
     <t>C4</t>
   </si>
   <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>T8</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>TP7</t>
+  </si>
+  <si>
+    <t>CP5</t>
+  </si>
+  <si>
+    <t>CP3</t>
+  </si>
+  <si>
+    <t>CP1</t>
+  </si>
+  <si>
+    <t>CPz</t>
+  </si>
+  <si>
+    <t>CP2</t>
+  </si>
+  <si>
+    <t>CP4</t>
+  </si>
+  <si>
+    <t>CP6</t>
+  </si>
+  <si>
+    <t>TP8</t>
+  </si>
+  <si>
+    <t>P9</t>
+  </si>
+  <si>
+    <t>P7</t>
+  </si>
+  <si>
+    <t>P5</t>
+  </si>
+  <si>
     <t>P3</t>
   </si>
   <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Pz</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
     <t>P4</t>
   </si>
   <si>
+    <t>P6</t>
+  </si>
+  <si>
+    <t>P8</t>
+  </si>
+  <si>
+    <t>P10</t>
+  </si>
+  <si>
+    <t>PO9</t>
+  </si>
+  <si>
+    <t>PO7</t>
+  </si>
+  <si>
+    <t>PO5</t>
+  </si>
+  <si>
+    <t>PO3</t>
+  </si>
+  <si>
+    <t>PO1</t>
+  </si>
+  <si>
+    <t>POz</t>
+  </si>
+  <si>
+    <t>PO2</t>
+  </si>
+  <si>
+    <t>PO4</t>
+  </si>
+  <si>
+    <t>PO6</t>
+  </si>
+  <si>
+    <t>PO8</t>
+  </si>
+  <si>
+    <t>PO10</t>
+  </si>
+  <si>
     <t>O1</t>
   </si>
   <si>
+    <t>Oz</t>
+  </si>
+  <si>
     <t>O2</t>
   </si>
   <si>
-    <t>F7</t>
-  </si>
-  <si>
-    <t>F8</t>
-  </si>
-  <si>
-    <t>T7</t>
-  </si>
-  <si>
-    <t>T8</t>
-  </si>
-  <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>P8</t>
-  </si>
-  <si>
-    <t>Fz</t>
-  </si>
-  <si>
-    <t>Cz</t>
-  </si>
-  <si>
-    <t>Pz</t>
-  </si>
-  <si>
-    <t>F1</t>
-  </si>
-  <si>
-    <t>F2</t>
-  </si>
-  <si>
-    <t>FC1</t>
-  </si>
-  <si>
-    <t>FC2</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>CP1</t>
-  </si>
-  <si>
-    <t>CP2</t>
-  </si>
-  <si>
-    <t>P1</t>
-  </si>
-  <si>
-    <t>P2</t>
-  </si>
-  <si>
-    <t>AF3</t>
-  </si>
-  <si>
-    <t>AF4</t>
-  </si>
-  <si>
-    <t>FC3</t>
-  </si>
-  <si>
-    <t>FC4</t>
-  </si>
-  <si>
-    <t>CP3</t>
-  </si>
-  <si>
-    <t>CP4</t>
-  </si>
-  <si>
-    <t>PO3</t>
-  </si>
-  <si>
-    <t>PO4</t>
-  </si>
-  <si>
-    <t>F5</t>
-  </si>
-  <si>
-    <t>F6</t>
-  </si>
-  <si>
-    <t>FC5</t>
-  </si>
-  <si>
-    <t>FC6</t>
-  </si>
-  <si>
-    <t>C5</t>
-  </si>
-  <si>
-    <t>C6</t>
-  </si>
-  <si>
-    <t>CP5</t>
-  </si>
-  <si>
-    <t>CP6</t>
-  </si>
-  <si>
-    <t>P5</t>
-  </si>
-  <si>
-    <t>P6</t>
-  </si>
-  <si>
-    <t>AF7</t>
-  </si>
-  <si>
-    <t>AF8</t>
-  </si>
-  <si>
-    <t>FT7</t>
-  </si>
-  <si>
-    <t>FT8</t>
-  </si>
-  <si>
-    <t>TP7</t>
-  </si>
-  <si>
-    <t>TP8</t>
-  </si>
-  <si>
-    <t>PO7</t>
-  </si>
-  <si>
-    <t>PO8</t>
-  </si>
-  <si>
-    <t>F9</t>
-  </si>
-  <si>
-    <t>F10</t>
-  </si>
-  <si>
-    <t>FT9</t>
-  </si>
-  <si>
-    <t>FT10</t>
-  </si>
-  <si>
-    <t>P9</t>
-  </si>
-  <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>PO9</t>
-  </si>
-  <si>
-    <t>PO10</t>
-  </si>
-  <si>
     <t>O9</t>
   </si>
   <si>
     <t>O10</t>
   </si>
   <si>
-    <t>Fpz</t>
-  </si>
-  <si>
-    <t>AFz</t>
-  </si>
-  <si>
-    <t>FCz</t>
-  </si>
-  <si>
-    <t>CPz</t>
-  </si>
-  <si>
-    <t>POz</t>
-  </si>
-  <si>
-    <t>Oz</t>
+    <t>I1</t>
   </si>
   <si>
     <t>Iz</t>
-  </si>
-  <si>
-    <t>LPA</t>
-  </si>
-  <si>
-    <t>RPA</t>
-  </si>
-  <si>
-    <t>Nz</t>
-  </si>
-  <si>
-    <t>AF5</t>
-  </si>
-  <si>
-    <t>AF1</t>
-  </si>
-  <si>
-    <t>AF2</t>
-  </si>
-  <si>
-    <t>AF6</t>
-  </si>
-  <si>
-    <t>T9</t>
-  </si>
-  <si>
-    <t>T10</t>
-  </si>
-  <si>
-    <t>PO5</t>
-  </si>
-  <si>
-    <t>PO1</t>
-  </si>
-  <si>
-    <t>PO2</t>
-  </si>
-  <si>
-    <t>PO6</t>
-  </si>
-  <si>
-    <t>I1</t>
   </si>
   <si>
     <t>I2</t>
@@ -3027,13 +3027,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="0">
-        <v>-0.30745244171826708</v>
+        <v>-0.86576871099802055</v>
       </c>
       <c r="C1" s="0">
-        <v>0.95039859019750939</v>
+        <v>1.0602608807256557e-16</v>
       </c>
       <c r="D1" s="0">
-        <v>-0.047069266321689091</v>
+        <v>-0.50044434161735296</v>
       </c>
     </row>
     <row r="2">
@@ -3041,13 +3041,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0">
-        <v>0.30745244171826697</v>
+        <v>0.86576871099802055</v>
       </c>
       <c r="C2" s="0">
-        <v>0.95039859019750939</v>
+        <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>-0.047069266321689091</v>
+        <v>-0.50044434161735296</v>
       </c>
     </row>
     <row r="3">
@@ -3055,13 +3055,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="0">
-        <v>-0.56706266388673054</v>
+        <v>5.5926998114099362e-17</v>
       </c>
       <c r="C3" s="0">
-        <v>0.67707482090179294</v>
+        <v>0.91335719250706271</v>
       </c>
       <c r="D3" s="0">
-        <v>0.46905183309149312</v>
+        <v>-0.40715923039471469</v>
       </c>
     </row>
     <row r="4">
@@ -3069,13 +3069,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="0">
-        <v>0.56638357156090047</v>
+        <v>-0.30745244171826708</v>
       </c>
       <c r="C4" s="0">
-        <v>0.67745879495888617</v>
+        <v>0.95039859019750939</v>
       </c>
       <c r="D4" s="0">
-        <v>0.46931783579869657</v>
+        <v>-0.047069266321689091</v>
       </c>
     </row>
     <row r="5">
@@ -3083,13 +3083,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="0">
-        <v>-0.74319453039520555</v>
+        <v>6.1218815664340533e-17</v>
       </c>
       <c r="C5" s="0">
-        <v>9.1015080279230885e-17</v>
+        <v>0.99977913153349129</v>
       </c>
       <c r="D5" s="0">
-        <v>0.66907539933153271</v>
+        <v>-0.021016378140343659</v>
       </c>
     </row>
     <row r="6">
@@ -3097,13 +3097,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="0">
-        <v>0.74314492739264038</v>
+        <v>0.30745244171826697</v>
       </c>
       <c r="C6" s="0">
-        <v>0</v>
+        <v>0.95039859019750939</v>
       </c>
       <c r="D6" s="0">
-        <v>0.66913049317049311</v>
+        <v>-0.047069266321689091</v>
       </c>
     </row>
     <row r="7">
@@ -3111,13 +3111,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="0">
-        <v>-0.56706266388673054</v>
+        <v>-0.58481785482806115</v>
       </c>
       <c r="C7" s="0">
-        <v>-0.67707482090179294</v>
+        <v>0.80813015213398198</v>
       </c>
       <c r="D7" s="0">
-        <v>0.46905183309149312</v>
+        <v>-0.0700980305444594</v>
       </c>
     </row>
     <row r="8">
@@ -3125,13 +3125,13 @@
         <v>7</v>
       </c>
       <c r="B8" s="0">
-        <v>0.56638357156090047</v>
+        <v>-0.50530681438277425</v>
       </c>
       <c r="C8" s="0">
-        <v>-0.67745879495888617</v>
+        <v>0.85652006556763272</v>
       </c>
       <c r="D8" s="0">
-        <v>0.46931783579869657</v>
+        <v>0.10506379308948768</v>
       </c>
     </row>
     <row r="9">
@@ -3139,13 +3139,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="0">
-        <v>-0.30745244171826708</v>
+        <v>-0.37037983409478908</v>
       </c>
       <c r="C9" s="0">
-        <v>-0.95039859019750939</v>
+        <v>0.89591878787793533</v>
       </c>
       <c r="D9" s="0">
-        <v>-0.047069266321689091</v>
+        <v>0.24525151176546833</v>
       </c>
     </row>
     <row r="10">
@@ -3153,13 +3153,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="0">
-        <v>0.30745244171826697</v>
+        <v>-0.19622460950348083</v>
       </c>
       <c r="C10" s="0">
-        <v>-0.95039859019750939</v>
+        <v>0.92105428950613444</v>
       </c>
       <c r="D10" s="0">
-        <v>-0.047069266321689091</v>
+        <v>0.33638504486310994</v>
       </c>
     </row>
     <row r="11">
@@ -3167,13 +3167,13 @@
         <v>10</v>
       </c>
       <c r="B11" s="0">
-        <v>-0.80498429257619908</v>
+        <v>5.6928553264966552e-17</v>
       </c>
       <c r="C11" s="0">
-        <v>0.58671740727568733</v>
+        <v>0.92971382940130043</v>
       </c>
       <c r="D11" s="0">
-        <v>-0.08810773351580288</v>
+        <v>0.36828276557554207</v>
       </c>
     </row>
     <row r="12">
@@ -3181,13 +3181,13 @@
         <v>11</v>
       </c>
       <c r="B12" s="0">
-        <v>0.80451142957190869</v>
+        <v>0.19508175638747935</v>
       </c>
       <c r="C12" s="0">
-        <v>0.587373394476008</v>
+        <v>0.92138614170701771</v>
       </c>
       <c r="D12" s="0">
-        <v>-0.088055977366079563</v>
+        <v>0.33614087254457975</v>
       </c>
     </row>
     <row r="13">
@@ -3195,13 +3195,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="0">
-        <v>-0.99457104771914984</v>
+        <v>0.37037983409478897</v>
       </c>
       <c r="C13" s="0">
-        <v>1.2179982501138862e-16</v>
+        <v>0.89591878787793533</v>
       </c>
       <c r="D13" s="0">
-        <v>-0.10405974744747643</v>
+        <v>0.24525151176546833</v>
       </c>
     </row>
     <row r="14">
@@ -3209,13 +3209,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="0">
-        <v>0.99457104771914984</v>
+        <v>0.50530681438277414</v>
       </c>
       <c r="C14" s="0">
-        <v>0</v>
+        <v>0.85652006556763272</v>
       </c>
       <c r="D14" s="0">
-        <v>-0.10405974744747643</v>
+        <v>0.10506379308948768</v>
       </c>
     </row>
     <row r="15">
@@ -3223,13 +3223,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="0">
-        <v>-0.80498429257619908</v>
+        <v>0.58434486523576323</v>
       </c>
       <c r="C15" s="0">
-        <v>-0.58671740727568733</v>
+        <v>0.80847714231249446</v>
       </c>
       <c r="D15" s="0">
-        <v>-0.08810773351580288</v>
+        <v>-0.070041336586478473</v>
       </c>
     </row>
     <row r="16">
@@ -3237,13 +3237,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="0">
-        <v>0.80451142957190869</v>
+        <v>-0.70247186834261666</v>
       </c>
       <c r="C16" s="0">
-        <v>-0.587373394476008</v>
+        <v>0.5233515486370206</v>
       </c>
       <c r="D16" s="0">
-        <v>-0.088055977366079563</v>
+        <v>-0.48232398937484511</v>
       </c>
     </row>
     <row r="17">
@@ -3251,13 +3251,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="0">
-        <v>4.3754974406970394e-17</v>
+        <v>-0.80498429257619908</v>
       </c>
       <c r="C17" s="0">
-        <v>0.71457295993317116</v>
+        <v>0.58671740727568733</v>
       </c>
       <c r="D17" s="0">
-        <v>0.69956092295978523</v>
+        <v>-0.08810773351580288</v>
       </c>
     </row>
     <row r="18">
@@ -3265,13 +3265,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="0">
-        <v>6.123233995736766e-17</v>
+        <v>-0.74186291750427535</v>
       </c>
       <c r="C18" s="0">
-        <v>0</v>
+        <v>0.63573947721351576</v>
       </c>
       <c r="D18" s="0">
-        <v>1</v>
+        <v>0.21324804511256504</v>
       </c>
     </row>
     <row r="19">
@@ -3279,13 +3279,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="0">
-        <v>4.3754974406970394e-17</v>
+        <v>-0.56706266388673054</v>
       </c>
       <c r="C19" s="0">
-        <v>-0.71457295993317116</v>
+        <v>0.67707482090179294</v>
       </c>
       <c r="D19" s="0">
-        <v>0.69956092295978523</v>
+        <v>0.46905183309149312</v>
       </c>
     </row>
     <row r="20">
@@ -3307,13 +3307,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="0">
-        <v>0.30617579537430567</v>
+        <v>4.3754974406970394e-17</v>
       </c>
       <c r="C21" s="0">
-        <v>0.7044044442598405</v>
+        <v>0.71457295993317116</v>
       </c>
       <c r="D21" s="0">
-        <v>0.64036767659985505</v>
+        <v>0.69956092295978523</v>
       </c>
     </row>
     <row r="22">
@@ -3321,13 +3321,13 @@
         <v>21</v>
       </c>
       <c r="B22" s="0">
-        <v>-0.38060144489772013</v>
+        <v>0.30617579537430567</v>
       </c>
       <c r="C22" s="0">
-        <v>0.38160302764745108</v>
+        <v>0.7044044442598405</v>
       </c>
       <c r="D22" s="0">
-        <v>0.84233109252363847</v>
+        <v>0.64036767659985505</v>
       </c>
     </row>
     <row r="23">
@@ -3335,13 +3335,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="0">
-        <v>0.38060144489772013</v>
+        <v>0.56638357156090047</v>
       </c>
       <c r="C23" s="0">
-        <v>0.38160302764745097</v>
+        <v>0.67745879495888617</v>
       </c>
       <c r="D23" s="0">
-        <v>0.84233109252363847</v>
+        <v>0.46931783579869657</v>
       </c>
     </row>
     <row r="24">
@@ -3349,13 +3349,13 @@
         <v>23</v>
       </c>
       <c r="B24" s="0">
-        <v>-0.40632417284334887</v>
+        <v>0.74170421160392219</v>
       </c>
       <c r="C24" s="0">
-        <v>-4.9760359768880312e-17</v>
+        <v>0.63560347418149876</v>
       </c>
       <c r="D24" s="0">
-        <v>0.91372898966989569</v>
+        <v>0.2142033755509303</v>
       </c>
     </row>
     <row r="25">
@@ -3363,13 +3363,13 @@
         <v>24</v>
       </c>
       <c r="B25" s="0">
-        <v>0.40715923039471458</v>
+        <v>0.80451142957190869</v>
       </c>
       <c r="C25" s="0">
-        <v>0</v>
+        <v>0.587373394476008</v>
       </c>
       <c r="D25" s="0">
-        <v>0.91335719250706282</v>
+        <v>-0.088055977366079563</v>
       </c>
     </row>
     <row r="26">
@@ -3377,13 +3377,13 @@
         <v>25</v>
       </c>
       <c r="B26" s="0">
-        <v>-0.38060144489772013</v>
+        <v>0.70247186834261655</v>
       </c>
       <c r="C26" s="0">
-        <v>-0.38160302764745108</v>
+        <v>0.52335154863702071</v>
       </c>
       <c r="D26" s="0">
-        <v>0.84233109252363847</v>
+        <v>-0.48232398937484511</v>
       </c>
     </row>
     <row r="27">
@@ -3391,13 +3391,13 @@
         <v>26</v>
       </c>
       <c r="B27" s="0">
-        <v>0.38060144489772013</v>
+        <v>-0.8243805394487046</v>
       </c>
       <c r="C27" s="0">
-        <v>-0.38160302764745097</v>
+        <v>0.27412653860308889</v>
       </c>
       <c r="D27" s="0">
-        <v>0.84233109252363847</v>
+        <v>-0.4952286007610544</v>
       </c>
     </row>
     <row r="28">
@@ -3405,13 +3405,13 @@
         <v>27</v>
       </c>
       <c r="B28" s="0">
-        <v>-0.30637200828520089</v>
+        <v>-0.94599902949198711</v>
       </c>
       <c r="C28" s="0">
-        <v>-0.70485586219863194</v>
+        <v>0.30832560961220318</v>
       </c>
       <c r="D28" s="0">
-        <v>0.63977684083086039</v>
+        <v>-0.10010571740655948</v>
       </c>
     </row>
     <row r="29">
@@ -3419,13 +3419,13 @@
         <v>28</v>
       </c>
       <c r="B29" s="0">
-        <v>0.30617579537430567</v>
+        <v>-0.8970249881392528</v>
       </c>
       <c r="C29" s="0">
-        <v>-0.7044044442598405</v>
+        <v>0.33838665847217353</v>
       </c>
       <c r="D29" s="0">
-        <v>0.64036767659985505</v>
+        <v>0.28432488463342392</v>
       </c>
     </row>
     <row r="30">
@@ -3433,13 +3433,13 @@
         <v>29</v>
       </c>
       <c r="B30" s="0">
-        <v>-0.37037983409478908</v>
+        <v>-0.6973508557428616</v>
       </c>
       <c r="C30" s="0">
-        <v>0.89591878787793533</v>
+        <v>0.36418323025882593</v>
       </c>
       <c r="D30" s="0">
-        <v>0.24525151176546833</v>
+        <v>0.61731058535630645</v>
       </c>
     </row>
     <row r="31">
@@ -3447,13 +3447,13 @@
         <v>30</v>
       </c>
       <c r="B31" s="0">
-        <v>0.37037983409478897</v>
+        <v>-0.38060144489772013</v>
       </c>
       <c r="C31" s="0">
-        <v>0.89591878787793533</v>
+        <v>0.38160302764745108</v>
       </c>
       <c r="D31" s="0">
-        <v>0.24525151176546833</v>
+        <v>0.84233109252363847</v>
       </c>
     </row>
     <row r="32">
@@ -3461,13 +3461,13 @@
         <v>31</v>
       </c>
       <c r="B32" s="0">
-        <v>-0.6973508557428616</v>
+        <v>2.3720529243755107e-17</v>
       </c>
       <c r="C32" s="0">
-        <v>0.36418323025882593</v>
+        <v>0.38738564066423498</v>
       </c>
       <c r="D32" s="0">
-        <v>0.61731058535630645</v>
+        <v>0.92191776499162892</v>
       </c>
     </row>
     <row r="33">
@@ -3475,13 +3475,13 @@
         <v>32</v>
       </c>
       <c r="B33" s="0">
-        <v>0.6973508557428616</v>
+        <v>0.38060144489772013</v>
       </c>
       <c r="C33" s="0">
-        <v>0.36418323025882587</v>
+        <v>0.38160302764745097</v>
       </c>
       <c r="D33" s="0">
-        <v>0.61731058535630645</v>
+        <v>0.84233109252363847</v>
       </c>
     </row>
     <row r="34">
@@ -3489,10 +3489,10 @@
         <v>33</v>
       </c>
       <c r="B34" s="0">
-        <v>-0.6973508557428616</v>
+        <v>0.6973508557428616</v>
       </c>
       <c r="C34" s="0">
-        <v>-0.36418323025882593</v>
+        <v>0.36418323025882587</v>
       </c>
       <c r="D34" s="0">
         <v>0.61731058535630645</v>
@@ -3503,13 +3503,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="0">
-        <v>0.6973508557428616</v>
+        <v>0.89702498813925291</v>
       </c>
       <c r="C35" s="0">
-        <v>-0.36418323025882587</v>
+        <v>0.33838665847217347</v>
       </c>
       <c r="D35" s="0">
-        <v>0.61731058535630645</v>
+        <v>0.28432488463342392</v>
       </c>
     </row>
     <row r="36">
@@ -3517,13 +3517,13 @@
         <v>35</v>
       </c>
       <c r="B36" s="0">
-        <v>-0.37037983409478908</v>
+        <v>0.94599902949198711</v>
       </c>
       <c r="C36" s="0">
-        <v>-0.89591878787793533</v>
+        <v>0.30832560961220318</v>
       </c>
       <c r="D36" s="0">
-        <v>0.24525151176546833</v>
+        <v>-0.10010571740655948</v>
       </c>
     </row>
     <row r="37">
@@ -3531,13 +3531,13 @@
         <v>36</v>
       </c>
       <c r="B37" s="0">
-        <v>0.37037983409478897</v>
+        <v>0.82438053944870471</v>
       </c>
       <c r="C37" s="0">
-        <v>-0.89591878787793533</v>
+        <v>0.27412653860308878</v>
       </c>
       <c r="D37" s="0">
-        <v>0.24525151176546833</v>
+        <v>-0.4952286007610544</v>
       </c>
     </row>
     <row r="38">
@@ -3545,13 +3545,13 @@
         <v>37</v>
       </c>
       <c r="B38" s="0">
-        <v>-0.74186291750427535</v>
+        <v>-0.86576871099802055</v>
       </c>
       <c r="C38" s="0">
-        <v>0.63573947721351576</v>
+        <v>1.0602608807256557e-16</v>
       </c>
       <c r="D38" s="0">
-        <v>0.21324804511256504</v>
+        <v>-0.50044434161735296</v>
       </c>
     </row>
     <row r="39">
@@ -3559,13 +3559,13 @@
         <v>38</v>
       </c>
       <c r="B39" s="0">
-        <v>0.74170421160392219</v>
+        <v>-0.99457104771914984</v>
       </c>
       <c r="C39" s="0">
-        <v>0.63560347418149876</v>
+        <v>1.2179982501138862e-16</v>
       </c>
       <c r="D39" s="0">
-        <v>0.2142033755509303</v>
+        <v>-0.10405974744747643</v>
       </c>
     </row>
     <row r="40">
@@ -3573,13 +3573,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="0">
-        <v>-0.8970249881392528</v>
+        <v>-0.95096047965126318</v>
       </c>
       <c r="C40" s="0">
-        <v>0.33838665847217353</v>
+        <v>1.1645907075205511e-16</v>
       </c>
       <c r="D40" s="0">
-        <v>0.28432488463342392</v>
+        <v>0.30931240864446347</v>
       </c>
     </row>
     <row r="41">
@@ -3587,13 +3587,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="0">
-        <v>0.89702498813925291</v>
+        <v>-0.74319453039520555</v>
       </c>
       <c r="C41" s="0">
-        <v>0.33838665847217347</v>
+        <v>9.1015080279230885e-17</v>
       </c>
       <c r="D41" s="0">
-        <v>0.28432488463342392</v>
+        <v>0.66907539933153271</v>
       </c>
     </row>
     <row r="42">
@@ -3601,13 +3601,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="0">
-        <v>-0.95096047965126318</v>
+        <v>-0.40632417284334887</v>
       </c>
       <c r="C42" s="0">
-        <v>1.1645907075205511e-16</v>
+        <v>-4.9760359768880312e-17</v>
       </c>
       <c r="D42" s="0">
-        <v>0.30931240864446347</v>
+        <v>0.91372898966989569</v>
       </c>
     </row>
     <row r="43">
@@ -3615,13 +3615,13 @@
         <v>42</v>
       </c>
       <c r="B43" s="0">
-        <v>0.95096047965126318</v>
+        <v>6.123233995736766e-17</v>
       </c>
       <c r="C43" s="0">
         <v>0</v>
       </c>
       <c r="D43" s="0">
-        <v>0.30931240864446347</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
@@ -3629,13 +3629,13 @@
         <v>43</v>
       </c>
       <c r="B44" s="0">
-        <v>-0.8970249881392528</v>
+        <v>0.40715923039471458</v>
       </c>
       <c r="C44" s="0">
-        <v>-0.33838665847217353</v>
+        <v>0</v>
       </c>
       <c r="D44" s="0">
-        <v>0.28432488463342392</v>
+        <v>0.91335719250706282</v>
       </c>
     </row>
     <row r="45">
@@ -3643,13 +3643,13 @@
         <v>44</v>
       </c>
       <c r="B45" s="0">
-        <v>0.89702498813925291</v>
+        <v>0.74314492739264038</v>
       </c>
       <c r="C45" s="0">
-        <v>-0.33838665847217347</v>
+        <v>0</v>
       </c>
       <c r="D45" s="0">
-        <v>0.28432488463342392</v>
+        <v>0.66913049317049311</v>
       </c>
     </row>
     <row r="46">
@@ -3657,13 +3657,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="0">
-        <v>-0.74186291750427535</v>
+        <v>0.95096047965126318</v>
       </c>
       <c r="C46" s="0">
-        <v>-0.63573947721351576</v>
+        <v>0</v>
       </c>
       <c r="D46" s="0">
-        <v>0.21324804511256504</v>
+        <v>0.30931240864446347</v>
       </c>
     </row>
     <row r="47">
@@ -3671,13 +3671,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="0">
-        <v>0.74170421160392219</v>
+        <v>0.99457104771914984</v>
       </c>
       <c r="C47" s="0">
-        <v>-0.63560347418149876</v>
+        <v>0</v>
       </c>
       <c r="D47" s="0">
-        <v>0.2142033755509303</v>
+        <v>-0.10405974744747643</v>
       </c>
     </row>
     <row r="48">
@@ -3685,13 +3685,13 @@
         <v>47</v>
       </c>
       <c r="B48" s="0">
-        <v>-0.58481785482806115</v>
+        <v>0.86576871099802055</v>
       </c>
       <c r="C48" s="0">
-        <v>0.80813015213398198</v>
+        <v>0</v>
       </c>
       <c r="D48" s="0">
-        <v>-0.0700980305444594</v>
+        <v>-0.50044434161735296</v>
       </c>
     </row>
     <row r="49">
@@ -3699,13 +3699,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="0">
-        <v>0.58434486523576323</v>
+        <v>-0.94599902949198711</v>
       </c>
       <c r="C49" s="0">
-        <v>0.80847714231249446</v>
+        <v>-0.30832560961220318</v>
       </c>
       <c r="D49" s="0">
-        <v>-0.070041336586478473</v>
+        <v>-0.10010571740655948</v>
       </c>
     </row>
     <row r="50">
@@ -3713,13 +3713,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="0">
-        <v>-0.94599902949198711</v>
+        <v>-0.8970249881392528</v>
       </c>
       <c r="C50" s="0">
-        <v>0.30832560961220318</v>
+        <v>-0.33838665847217353</v>
       </c>
       <c r="D50" s="0">
-        <v>-0.10010571740655948</v>
+        <v>0.28432488463342392</v>
       </c>
     </row>
     <row r="51">
@@ -3727,13 +3727,13 @@
         <v>50</v>
       </c>
       <c r="B51" s="0">
-        <v>0.94599902949198711</v>
+        <v>-0.6973508557428616</v>
       </c>
       <c r="C51" s="0">
-        <v>0.30832560961220318</v>
+        <v>-0.36418323025882593</v>
       </c>
       <c r="D51" s="0">
-        <v>-0.10010571740655948</v>
+        <v>0.61731058535630645</v>
       </c>
     </row>
     <row r="52">
@@ -3741,13 +3741,13 @@
         <v>51</v>
       </c>
       <c r="B52" s="0">
-        <v>-0.94599902949198711</v>
+        <v>-0.38060144489772013</v>
       </c>
       <c r="C52" s="0">
-        <v>-0.30832560961220318</v>
+        <v>-0.38160302764745108</v>
       </c>
       <c r="D52" s="0">
-        <v>-0.10010571740655948</v>
+        <v>0.84233109252363847</v>
       </c>
     </row>
     <row r="53">
@@ -3755,13 +3755,13 @@
         <v>52</v>
       </c>
       <c r="B53" s="0">
-        <v>0.94570670696381387</v>
+        <v>2.3720529243755107e-17</v>
       </c>
       <c r="C53" s="0">
-        <v>-0.30923108195959625</v>
+        <v>-0.38738564066423498</v>
       </c>
       <c r="D53" s="0">
-        <v>-0.10007478380569458</v>
+        <v>0.92191776499162892</v>
       </c>
     </row>
     <row r="54">
@@ -3769,13 +3769,13 @@
         <v>53</v>
       </c>
       <c r="B54" s="0">
-        <v>-0.58481785482806115</v>
+        <v>0.38060144489772013</v>
       </c>
       <c r="C54" s="0">
-        <v>-0.80813015213398198</v>
+        <v>-0.38160302764745097</v>
       </c>
       <c r="D54" s="0">
-        <v>-0.0700980305444594</v>
+        <v>0.84233109252363847</v>
       </c>
     </row>
     <row r="55">
@@ -3783,13 +3783,13 @@
         <v>54</v>
       </c>
       <c r="B55" s="0">
-        <v>0.58434486523576323</v>
+        <v>0.6973508557428616</v>
       </c>
       <c r="C55" s="0">
-        <v>-0.80847714231249446</v>
+        <v>-0.36418323025882587</v>
       </c>
       <c r="D55" s="0">
-        <v>-0.070041336586478473</v>
+        <v>0.61731058535630645</v>
       </c>
     </row>
     <row r="56">
@@ -3797,13 +3797,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="0">
-        <v>-0.70247186834261666</v>
+        <v>0.89702498813925291</v>
       </c>
       <c r="C56" s="0">
-        <v>0.5233515486370206</v>
+        <v>-0.33838665847217347</v>
       </c>
       <c r="D56" s="0">
-        <v>-0.48232398937484511</v>
+        <v>0.28432488463342392</v>
       </c>
     </row>
     <row r="57">
@@ -3811,13 +3811,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="0">
-        <v>0.70247186834261655</v>
+        <v>0.94570670696381387</v>
       </c>
       <c r="C57" s="0">
-        <v>0.52335154863702071</v>
+        <v>-0.30923108195959625</v>
       </c>
       <c r="D57" s="0">
-        <v>-0.48232398937484511</v>
+        <v>-0.10007478380569458</v>
       </c>
     </row>
     <row r="58">
@@ -3825,13 +3825,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="0">
-        <v>-0.8243805394487046</v>
+        <v>-0.70247186834261666</v>
       </c>
       <c r="C58" s="0">
-        <v>0.27412653860308889</v>
+        <v>-0.5233515486370206</v>
       </c>
       <c r="D58" s="0">
-        <v>-0.4952286007610544</v>
+        <v>-0.48232398937484511</v>
       </c>
     </row>
     <row r="59">
@@ -3839,13 +3839,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="0">
-        <v>0.82438053944870471</v>
+        <v>-0.80498429257619908</v>
       </c>
       <c r="C59" s="0">
-        <v>0.27412653860308878</v>
+        <v>-0.58671740727568733</v>
       </c>
       <c r="D59" s="0">
-        <v>-0.4952286007610544</v>
+        <v>-0.08810773351580288</v>
       </c>
     </row>
     <row r="60">
@@ -3853,13 +3853,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="0">
-        <v>-0.70247186834261666</v>
+        <v>-0.74186291750427535</v>
       </c>
       <c r="C60" s="0">
-        <v>-0.5233515486370206</v>
+        <v>-0.63573947721351576</v>
       </c>
       <c r="D60" s="0">
-        <v>-0.48232398937484511</v>
+        <v>0.21324804511256504</v>
       </c>
     </row>
     <row r="61">
@@ -3867,13 +3867,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="0">
-        <v>0.70247186834261655</v>
+        <v>-0.56706266388673054</v>
       </c>
       <c r="C61" s="0">
-        <v>-0.52335154863702071</v>
+        <v>-0.67707482090179294</v>
       </c>
       <c r="D61" s="0">
-        <v>-0.48232398937484511</v>
+        <v>0.46905183309149312</v>
       </c>
     </row>
     <row r="62">
@@ -3881,13 +3881,13 @@
         <v>61</v>
       </c>
       <c r="B62" s="0">
-        <v>-0.51243139260174553</v>
+        <v>-0.30637200828520089</v>
       </c>
       <c r="C62" s="0">
-        <v>-0.72360917353723053</v>
+        <v>-0.70485586219863194</v>
       </c>
       <c r="D62" s="0">
-        <v>-0.46238926441798134</v>
+        <v>0.63977684083086039</v>
       </c>
     </row>
     <row r="63">
@@ -3895,13 +3895,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="0">
-        <v>0.51206042669573559</v>
+        <v>4.3754974406970394e-17</v>
       </c>
       <c r="C63" s="0">
-        <v>-0.72408544712443856</v>
+        <v>-0.71457295993317116</v>
       </c>
       <c r="D63" s="0">
-        <v>-0.46205452565123006</v>
+        <v>0.69956092295978523</v>
       </c>
     </row>
     <row r="64">
@@ -3909,13 +3909,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="0">
-        <v>-0.2701134714920464</v>
+        <v>0.30617579537430567</v>
       </c>
       <c r="C64" s="0">
-        <v>-0.85836058718583563</v>
+        <v>-0.7044044442598405</v>
       </c>
       <c r="D64" s="0">
-        <v>-0.43618323544641535</v>
+        <v>0.64036767659985505</v>
       </c>
     </row>
     <row r="65">
@@ -3923,13 +3923,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="0">
-        <v>0.27011347149204634</v>
+        <v>0.56638357156090047</v>
       </c>
       <c r="C65" s="0">
-        <v>-0.85836058718583563</v>
+        <v>-0.67745879495888617</v>
       </c>
       <c r="D65" s="0">
-        <v>-0.43618323544641535</v>
+        <v>0.46931783579869657</v>
       </c>
     </row>
     <row r="66">
@@ -3937,13 +3937,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="0">
-        <v>6.1218815664340533e-17</v>
+        <v>0.74170421160392219</v>
       </c>
       <c r="C66" s="0">
-        <v>0.99977913153349129</v>
+        <v>-0.63560347418149876</v>
       </c>
       <c r="D66" s="0">
-        <v>-0.021016378140343659</v>
+        <v>0.2142033755509303</v>
       </c>
     </row>
     <row r="67">
@@ -3951,13 +3951,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="0">
-        <v>5.6928553264966552e-17</v>
+        <v>0.80451142957190869</v>
       </c>
       <c r="C67" s="0">
-        <v>0.92971382940130043</v>
+        <v>-0.587373394476008</v>
       </c>
       <c r="D67" s="0">
-        <v>0.36828276557554207</v>
+        <v>-0.088055977366079563</v>
       </c>
     </row>
     <row r="68">
@@ -3965,13 +3965,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="0">
-        <v>2.3720529243755107e-17</v>
+        <v>0.70247186834261655</v>
       </c>
       <c r="C68" s="0">
-        <v>0.38738564066423498</v>
+        <v>-0.52335154863702071</v>
       </c>
       <c r="D68" s="0">
-        <v>0.92191776499162892</v>
+        <v>-0.48232398937484511</v>
       </c>
     </row>
     <row r="69">
@@ -3979,13 +3979,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="0">
-        <v>2.3720529243755107e-17</v>
+        <v>-0.51243139260174553</v>
       </c>
       <c r="C69" s="0">
-        <v>-0.38738564066423498</v>
+        <v>-0.72360917353723053</v>
       </c>
       <c r="D69" s="0">
-        <v>0.92191776499162892</v>
+        <v>-0.46238926441798134</v>
       </c>
     </row>
     <row r="70">
@@ -3993,13 +3993,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="0">
-        <v>5.6928553264966552e-17</v>
+        <v>-0.58481785482806115</v>
       </c>
       <c r="C70" s="0">
-        <v>-0.92971382940130043</v>
+        <v>-0.80813015213398198</v>
       </c>
       <c r="D70" s="0">
-        <v>0.36828276557554207</v>
+        <v>-0.0700980305444594</v>
       </c>
     </row>
     <row r="71">
@@ -4007,13 +4007,13 @@
         <v>70</v>
       </c>
       <c r="B71" s="0">
-        <v>6.1218815664340533e-17</v>
+        <v>-0.50530681438277425</v>
       </c>
       <c r="C71" s="0">
-        <v>-0.99977913153349129</v>
+        <v>-0.85652006556763272</v>
       </c>
       <c r="D71" s="0">
-        <v>-0.021016378140343659</v>
+        <v>0.10506379308948768</v>
       </c>
     </row>
     <row r="72">
@@ -4021,13 +4021,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="0">
-        <v>5.5926998114099362e-17</v>
+        <v>-0.37037983409478908</v>
       </c>
       <c r="C72" s="0">
-        <v>-0.91335719250706271</v>
+        <v>-0.89591878787793533</v>
       </c>
       <c r="D72" s="0">
-        <v>-0.40715923039471469</v>
+        <v>0.24525151176546833</v>
       </c>
     </row>
     <row r="73">
@@ -4035,13 +4035,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="0">
-        <v>-0.86576871099802055</v>
+        <v>-0.19622460950348083</v>
       </c>
       <c r="C73" s="0">
-        <v>1.0602608807256557e-16</v>
+        <v>-0.92105428950613444</v>
       </c>
       <c r="D73" s="0">
-        <v>-0.50044434161735296</v>
+        <v>0.33638504486310994</v>
       </c>
     </row>
     <row r="74">
@@ -4049,13 +4049,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="0">
-        <v>0.86576871099802055</v>
+        <v>5.6928553264966552e-17</v>
       </c>
       <c r="C74" s="0">
-        <v>0</v>
+        <v>-0.92971382940130043</v>
       </c>
       <c r="D74" s="0">
-        <v>-0.50044434161735296</v>
+        <v>0.36828276557554207</v>
       </c>
     </row>
     <row r="75">
@@ -4063,13 +4063,13 @@
         <v>74</v>
       </c>
       <c r="B75" s="0">
-        <v>5.5926998114099362e-17</v>
+        <v>0.19508175638747935</v>
       </c>
       <c r="C75" s="0">
-        <v>0.91335719250706271</v>
+        <v>-0.92138614170701771</v>
       </c>
       <c r="D75" s="0">
-        <v>-0.40715923039471469</v>
+        <v>0.33614087254457975</v>
       </c>
     </row>
     <row r="76">
@@ -4077,13 +4077,13 @@
         <v>75</v>
       </c>
       <c r="B76" s="0">
-        <v>-0.50530681438277425</v>
+        <v>0.37037983409478897</v>
       </c>
       <c r="C76" s="0">
-        <v>0.85652006556763272</v>
+        <v>-0.89591878787793533</v>
       </c>
       <c r="D76" s="0">
-        <v>0.10506379308948768</v>
+        <v>0.24525151176546833</v>
       </c>
     </row>
     <row r="77">
@@ -4091,13 +4091,13 @@
         <v>76</v>
       </c>
       <c r="B77" s="0">
-        <v>-0.19622460950348083</v>
+        <v>0.50530681438277414</v>
       </c>
       <c r="C77" s="0">
-        <v>0.92105428950613444</v>
+        <v>-0.85652006556763272</v>
       </c>
       <c r="D77" s="0">
-        <v>0.33638504486310994</v>
+        <v>0.10506379308948768</v>
       </c>
     </row>
     <row r="78">
@@ -4105,13 +4105,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="0">
-        <v>0.19508175638747935</v>
+        <v>0.58434486523576323</v>
       </c>
       <c r="C78" s="0">
-        <v>0.92138614170701771</v>
+        <v>-0.80847714231249446</v>
       </c>
       <c r="D78" s="0">
-        <v>0.33614087254457975</v>
+        <v>-0.070041336586478473</v>
       </c>
     </row>
     <row r="79">
@@ -4119,13 +4119,13 @@
         <v>78</v>
       </c>
       <c r="B79" s="0">
-        <v>0.50530681438277414</v>
+        <v>0.51206042669573559</v>
       </c>
       <c r="C79" s="0">
-        <v>0.85652006556763272</v>
+        <v>-0.72408544712443856</v>
       </c>
       <c r="D79" s="0">
-        <v>0.10506379308948768</v>
+        <v>-0.46205452565123006</v>
       </c>
     </row>
     <row r="80">
@@ -4133,13 +4133,13 @@
         <v>79</v>
       </c>
       <c r="B80" s="0">
-        <v>-0.86576871099802055</v>
+        <v>-0.30745244171826708</v>
       </c>
       <c r="C80" s="0">
-        <v>1.0602608807256557e-16</v>
+        <v>-0.95039859019750939</v>
       </c>
       <c r="D80" s="0">
-        <v>-0.50044434161735296</v>
+        <v>-0.047069266321689091</v>
       </c>
     </row>
     <row r="81">
@@ -4147,13 +4147,13 @@
         <v>80</v>
       </c>
       <c r="B81" s="0">
-        <v>0.86576871099802055</v>
+        <v>6.1218815664340533e-17</v>
       </c>
       <c r="C81" s="0">
-        <v>0</v>
+        <v>-0.99977913153349129</v>
       </c>
       <c r="D81" s="0">
-        <v>-0.50044434161735296</v>
+        <v>-0.021016378140343659</v>
       </c>
     </row>
     <row r="82">
@@ -4161,13 +4161,13 @@
         <v>81</v>
       </c>
       <c r="B82" s="0">
-        <v>-0.50530681438277425</v>
+        <v>0.30745244171826697</v>
       </c>
       <c r="C82" s="0">
-        <v>-0.85652006556763272</v>
+        <v>-0.95039859019750939</v>
       </c>
       <c r="D82" s="0">
-        <v>0.10506379308948768</v>
+        <v>-0.047069266321689091</v>
       </c>
     </row>
     <row r="83">
@@ -4175,13 +4175,13 @@
         <v>82</v>
       </c>
       <c r="B83" s="0">
-        <v>-0.19622460950348083</v>
+        <v>-0.2701134714920464</v>
       </c>
       <c r="C83" s="0">
-        <v>-0.92105428950613444</v>
+        <v>-0.85836058718583563</v>
       </c>
       <c r="D83" s="0">
-        <v>0.33638504486310994</v>
+        <v>-0.43618323544641535</v>
       </c>
     </row>
     <row r="84">
@@ -4189,13 +4189,13 @@
         <v>83</v>
       </c>
       <c r="B84" s="0">
-        <v>0.19508175638747935</v>
+        <v>0.27011347149204634</v>
       </c>
       <c r="C84" s="0">
-        <v>-0.92138614170701771</v>
+        <v>-0.85836058718583563</v>
       </c>
       <c r="D84" s="0">
-        <v>0.33614087254457975</v>
+        <v>-0.43618323544641535</v>
       </c>
     </row>
     <row r="85">
@@ -4203,13 +4203,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="0">
-        <v>0.50530681438277414</v>
+        <v>-0.2701134714920464</v>
       </c>
       <c r="C85" s="0">
-        <v>-0.85652006556763272</v>
+        <v>-0.85836058718583563</v>
       </c>
       <c r="D85" s="0">
-        <v>0.10506379308948768</v>
+        <v>-0.43618323544641535</v>
       </c>
     </row>
     <row r="86">
@@ -4217,13 +4217,13 @@
         <v>85</v>
       </c>
       <c r="B86" s="0">
-        <v>-0.2701134714920464</v>
+        <v>5.5926998114099362e-17</v>
       </c>
       <c r="C86" s="0">
-        <v>-0.85836058718583563</v>
+        <v>-0.91335719250706271</v>
       </c>
       <c r="D86" s="0">
-        <v>-0.43618323544641535</v>
+        <v>-0.40715923039471469</v>
       </c>
     </row>
     <row r="87">

</xml_diff>